<commit_message>
excel --> txt 完结
</commit_message>
<xml_diff>
--- a/src/services/tool/Book1.xlsx
+++ b/src/services/tool/Book1.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="true"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="测试" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -321,7 +321,7 @@
 <worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -339,7 +339,7 @@
 <worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1"/>

</xml_diff>